<commit_message>
added recording method and saving data in excel file
</commit_message>
<xml_diff>
--- a/FaceBook/FaceBook/usersDB.xlsx
+++ b/FaceBook/FaceBook/usersDB.xlsx
@@ -15,8 +15,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Автор</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Автор:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1 - ж
+2 - м</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Имя</t>
   </si>
@@ -48,9 +83,6 @@
     <t>mail@mail.ru</t>
   </si>
   <si>
-    <t>qweqwr12312</t>
-  </si>
-  <si>
     <t>Имя2</t>
   </si>
   <si>
@@ -73,18 +105,6 @@
   </si>
   <si>
     <t>Фамилия5</t>
-  </si>
-  <si>
-    <t>qweqwr12313</t>
-  </si>
-  <si>
-    <t>qweqwr12314</t>
-  </si>
-  <si>
-    <t>qweqwr12315</t>
-  </si>
-  <si>
-    <t>qweqwr12316</t>
   </si>
   <si>
     <t>mail1@mail.ru</t>
@@ -103,7 +123,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +138,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -446,11 +479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,9 +532,6 @@
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" s="2">
         <v>42370</v>
       </c>
@@ -515,16 +545,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2">
         <v>42371</v>
@@ -535,20 +562,17 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A13" si="0">1+A3</f>
+        <f t="shared" ref="A4:A6" si="0">1+A3</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="2">
         <v>42372</v>
@@ -563,16 +587,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2">
         <v>42373</v>
@@ -587,16 +608,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2">
         <v>42374</v>
@@ -615,6 +633,7 @@
     <hyperlink ref="D5" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
attach edit excel file
</commit_message>
<xml_diff>
--- a/FaceBook/FaceBook/usersDB.xlsx
+++ b/FaceBook/FaceBook/usersDB.xlsx
@@ -15,43 +15,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Автор</author>
-  </authors>
-  <commentList>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Автор:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-1 - ж
-2 - м</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Имя</t>
   </si>
@@ -74,56 +39,29 @@
     <t>Номер</t>
   </si>
   <si>
-    <t>Имя1</t>
-  </si>
-  <si>
-    <t>Фамилия1</t>
-  </si>
-  <si>
-    <t>mail@mail.ru</t>
-  </si>
-  <si>
-    <t>Имя2</t>
-  </si>
-  <si>
-    <t>Имя3</t>
-  </si>
-  <si>
-    <t>Имя4</t>
-  </si>
-  <si>
-    <t>Имя5</t>
-  </si>
-  <si>
-    <t>Фамилия2</t>
-  </si>
-  <si>
-    <t>Фамилия3</t>
-  </si>
-  <si>
-    <t>Фамилия4</t>
-  </si>
-  <si>
-    <t>Фамилия5</t>
-  </si>
-  <si>
-    <t>mail1@mail.ru</t>
-  </si>
-  <si>
-    <t>mail2@mail.ru</t>
-  </si>
-  <si>
-    <t>mail3@mail.ru</t>
-  </si>
-  <si>
-    <t>mail4@mail.ru</t>
+    <t>petya-pervyy-1999@mail.ru</t>
+  </si>
+  <si>
+    <t>Петр</t>
+  </si>
+  <si>
+    <t>Жигулёвский</t>
+  </si>
+  <si>
+    <t>nWE#w(Qb</t>
+  </si>
+  <si>
+    <t>Пароль от электронной почты</t>
+  </si>
+  <si>
+    <t>ntvyjnf123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,19 +76,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -479,11 +404,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E6" sqref="E3:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,10 +418,11 @@
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -513,127 +439,62 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2">
-        <v>42370</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2">
+        <v>32874</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>1+A2</f>
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2">
-        <v>42371</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+      <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f t="shared" ref="A4:A6" si="0">1+A3</f>
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2">
-        <v>42372</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+      <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="2">
-        <v>42373</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+      <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="2">
-        <v>42374</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+      <c r="F6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3:D6" r:id="rId2" display="mail@mail.ru"/>
-    <hyperlink ref="D3" r:id="rId3"/>
-    <hyperlink ref="D4" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D5" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added method recording in excel
</commit_message>
<xml_diff>
--- a/FaceBook/FaceBook/usersDB.xlsx
+++ b/FaceBook/FaceBook/usersDB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Имя</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>ntvyjnf123</t>
+  </si>
+  <si>
+    <t>Зарегистрирован</t>
+  </si>
+  <si>
+    <t>Марина</t>
+  </si>
+  <si>
+    <t>Шарапова</t>
+  </si>
+  <si>
+    <t>mail@mail.ru</t>
+  </si>
+  <si>
+    <t>fsdfsdfs</t>
+  </si>
+  <si>
+    <t>u3'*OlGq</t>
   </si>
 </sst>
 </file>
@@ -405,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E3:E6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,9 +438,10 @@
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -447,8 +466,11 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -473,26 +495,55 @@
       <c r="H2">
         <v>2</v>
       </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D3" s="1"/>
-      <c r="F3" s="2"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2">
+        <v>7337</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
       <c r="F6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
has been added model return error
</commit_message>
<xml_diff>
--- a/FaceBook/FaceBook/usersDB.xlsx
+++ b/FaceBook/FaceBook/usersDB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Имя</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>u3'*OlGq</t>
+  </si>
+  <si>
+    <t>Текст ошибки</t>
   </si>
 </sst>
 </file>
@@ -117,10 +120,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -423,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,9 +445,10 @@
     <col min="6" max="6" width="33" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -469,81 +476,75 @@
       <c r="I1" t="s">
         <v>13</v>
       </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="G2" s="2">
-        <v>32874</v>
+        <v>7337</v>
       </c>
       <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
       </c>
       <c r="G3" s="2">
-        <v>7337</v>
+        <v>32874</v>
       </c>
       <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
       <c r="F6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added recording homepage url in excel
</commit_message>
<xml_diff>
--- a/FaceBook/FaceBook/usersDB.xlsx
+++ b/FaceBook/FaceBook/usersDB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Имя</t>
   </si>
@@ -61,13 +61,19 @@
   </si>
   <si>
     <t>Текст ошибки</t>
+  </si>
+  <si>
+    <t>Домашняя с траница</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100013532889680</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +87,32 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -105,11 +137,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -414,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,46 +461,50 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="5" max="5" width="17" style="5" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="25.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -478,7 +517,7 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F2" t="s">
@@ -490,18 +529,21 @@
       <c r="H2">
         <v>2</v>
       </c>
-      <c r="I2" t="b">
-        <v>0</v>
+      <c r="I2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J3" s="3"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J3" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
       <c r="F6" s="2"/>
     </row>
@@ -510,6 +552,7 @@
     <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added parser excel file
</commit_message>
<xml_diff>
--- a/FaceBook/FaceBook/usersDB.xlsx
+++ b/FaceBook/FaceBook/usersDB.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Пользователи" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Информация о пользователях" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Имя</t>
   </si>
@@ -67,6 +67,93 @@
   </si>
   <si>
     <t>https://www.facebook.com/profile.php?id=100013532889680</t>
+  </si>
+  <si>
+    <t>Компания</t>
+  </si>
+  <si>
+    <t>Должность</t>
+  </si>
+  <si>
+    <t>Город</t>
+  </si>
+  <si>
+    <t>Умения и навыки</t>
+  </si>
+  <si>
+    <t>Школа</t>
+  </si>
+  <si>
+    <t>Описание (Работа)</t>
+  </si>
+  <si>
+    <t>Описание(Школа)</t>
+  </si>
+  <si>
+    <t>Специализации</t>
+  </si>
+  <si>
+    <t>ВУЗ</t>
+  </si>
+  <si>
+    <t>Описание(ВУЗ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id </t>
+  </si>
+  <si>
+    <t>СШ №3</t>
+  </si>
+  <si>
+    <t>лаборант</t>
+  </si>
+  <si>
+    <t>Москва</t>
+  </si>
+  <si>
+    <t>Умею всё!</t>
+  </si>
+  <si>
+    <t>МВЭИ</t>
+  </si>
+  <si>
+    <t>описание работы</t>
+  </si>
+  <si>
+    <t>описание вуза</t>
+  </si>
+  <si>
+    <t>экономист</t>
+  </si>
+  <si>
+    <t>Описание школы</t>
+  </si>
+  <si>
+    <t>СШ№2</t>
+  </si>
+  <si>
+    <t>СШ №2</t>
+  </si>
+  <si>
+    <t>учитель</t>
+  </si>
+  <si>
+    <t>Питер</t>
+  </si>
+  <si>
+    <t>Лучшая школа</t>
+  </si>
+  <si>
+    <t>токарь</t>
+  </si>
+  <si>
+    <t>МГИО</t>
+  </si>
+  <si>
+    <t>мгио вуз</t>
+  </si>
+  <si>
+    <t>Детсад №3</t>
   </si>
 </sst>
 </file>
@@ -137,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -145,6 +232,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -451,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,13 +648,132 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
edited Fiiling engine. fix bugs. added description errors file
</commit_message>
<xml_diff>
--- a/FaceBook/FaceBook/usersDB.xlsx
+++ b/FaceBook/FaceBook/usersDB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Пользователи" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Имя</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Описание школы</t>
   </si>
   <si>
-    <t>СШ№2</t>
-  </si>
-  <si>
     <t>СШ №2</t>
   </si>
   <si>
@@ -181,6 +178,18 @@
   </si>
   <si>
     <t>Семейное положение</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100013637047044</t>
+  </si>
+  <si>
+    <t>Город(ВУЗ)</t>
+  </si>
+  <si>
+    <t>Город(школа)</t>
+  </si>
+  <si>
+    <t>сш №209</t>
   </si>
 </sst>
 </file>
@@ -577,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I3"/>
     </sheetView>
   </sheetViews>
@@ -635,19 +644,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="G2" s="2">
         <v>31474</v>
@@ -655,7 +664,13 @@
       <c r="H2">
         <v>1</v>
       </c>
+      <c r="I2" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="J2" s="6"/>
+      <c r="K2" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
@@ -705,10 +720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,12 +735,16 @@
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="29.140625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="7" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>26</v>
       </c>
@@ -748,28 +767,34 @@
         <v>24</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>54</v>
+      <c r="P1" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -786,74 +811,86 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
       <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
       <c r="K2" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s">
         <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2">
+        <v>33</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>38</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>39</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
         <v>40</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
         <v>41</v>
       </c>
-      <c r="I3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
         <v>33</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" t="s">
         <v>52</v>
       </c>
-      <c r="M3" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3">
+      <c r="P3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added status registration model
</commit_message>
<xml_diff>
--- a/FaceBook/FaceBook/usersDB.xlsx
+++ b/FaceBook/FaceBook/usersDB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Пользователи" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>Имя</t>
   </si>
@@ -190,6 +190,24 @@
   </si>
   <si>
     <t>сш №209</t>
+  </si>
+  <si>
+    <t>Настоящий</t>
+  </si>
+  <si>
+    <t>Степан</t>
+  </si>
+  <si>
+    <t>nastoyashchiy.70@mail.ru</t>
+  </si>
+  <si>
+    <t>Si&gt;&amp;szo_</t>
+  </si>
+  <si>
+    <t>Код ошибки</t>
+  </si>
+  <si>
+    <t>Используйте телефон для подтверждения своего аккаунта.</t>
   </si>
 </sst>
 </file>
@@ -584,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,10 +619,11 @@
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" style="5" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -633,85 +652,126 @@
         <v>13</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>46</v>
       </c>
       <c r="G2" s="2">
+        <v>25785</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="2">
         <v>31474</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="I2" s="5" t="b">
+      <c r="I3" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="5" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="10">
+        <v>32874</v>
+      </c>
+      <c r="H4" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="10">
-        <v>32874</v>
-      </c>
-      <c r="H3" s="8">
-        <v>2</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D5" s="1"/>
-      <c r="F5" s="2"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
       <c r="F6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -720,10 +780,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,6 +954,56 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>